<commit_message>
Nils: Klasse Database in Projekt eingepflegt Pathfinding: - an Datenbankarbeit angepasst Node: - an Datenbankarbeit angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
+    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -326,40 +326,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A1: Problem Singeltouch lösen
-A2: Ebenen von Haus 5 und einem weiteren Haus grafisch darstellen
-A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
-    </r>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
     <t>A1: csv dateien für Haus 1, 2 und 3 anlegen (Knoten eintragen)</t>
-  </si>
-  <si>
-    <t>A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe</t>
   </si>
   <si>
     <t>A1: Modultests duchführen</t>
@@ -447,16 +417,66 @@
 A3: Startbildschirm entwerfen</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Problem Singeltouch lösen
+A2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ebenen von Haus 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">und einem weiteren Haus grafisch darstellen
+A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
+    </r>
+  </si>
+  <si>
+    <t>A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
+A2: Datenbank in UASJ-Maps bringen
+A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -913,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1078,6 +1098,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1096,15 +1143,6 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1114,23 +1152,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,7 +1244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1289,6 +1318,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1323,6 +1353,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1498,27 +1529,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1532,9 +1563,9 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1">
+    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1552,7 +1583,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1562,7 +1593,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1580,7 +1611,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1591,14 +1622,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="82"/>
-      <c r="H6" s="83"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="22.5">
+    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1609,14 +1640,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="78" t="s">
+      <c r="F7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="80"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1627,14 +1658,14 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1645,14 +1676,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="F9" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="47"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1663,14 +1694,14 @@
       <c r="E10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="78" t="s">
+      <c r="F10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="79"/>
-      <c r="H10" s="80"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1681,42 +1712,42 @@
       <c r="E11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="79"/>
-      <c r="H11" s="80"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="79"/>
-      <c r="H12" s="80"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="71"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1726,7 +1757,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1749,7 +1780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1760,14 +1791,14 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="101.25">
+    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
@@ -1778,32 +1809,32 @@
       <c r="E17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="74"/>
+      <c r="F17" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="146.25">
+    <row r="18" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="72" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="73"/>
-      <c r="H18" s="74"/>
+      <c r="F18" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="85"/>
+      <c r="H18" s="86"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="45">
+    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1814,32 +1845,32 @@
       <c r="E19" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="72" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
+      <c r="F19" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="101.25">
+    <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
       <c r="B20" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="73"/>
-      <c r="H20" s="74"/>
+      <c r="F20" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="45">
+    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="B21" s="58" t="s">
         <v>48</v>
       </c>
@@ -1848,16 +1879,16 @@
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="72" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="74"/>
+        <v>56</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="22.5">
+    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="48" t="s">
         <v>36</v>
       </c>
@@ -1866,16 +1897,16 @@
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="72" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1">
+    <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="48" t="s">
         <v>50</v>
       </c>
@@ -1886,14 +1917,14 @@
       <c r="E23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
+      <c r="F23" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="26"/>
@@ -1903,7 +1934,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="39" t="s">
         <v>3</v>
       </c>
@@ -1926,7 +1957,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="44" t="s">
         <v>5</v>
       </c>
@@ -1937,14 +1968,14 @@
       <c r="E26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="48" t="s">
         <v>6</v>
       </c>
@@ -1953,12 +1984,12 @@
       <c r="E27" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="75"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="77"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="83"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="48" t="s">
         <v>7</v>
       </c>
@@ -1967,12 +1998,12 @@
       <c r="E28" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="48" t="s">
         <v>8</v>
       </c>
@@ -1981,21 +2012,21 @@
       <c r="E29" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="68"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="77"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="59" t="s">
         <v>27</v>
       </c>
@@ -2003,7 +2034,7 @@
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
     </row>
-    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="59" t="s">
         <v>47</v>
       </c>
@@ -2013,7 +2044,7 @@
       <c r="H34" s="53"/>
       <c r="I34" s="54"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="59" t="s">
         <v>28</v>
       </c>
@@ -2023,7 +2054,7 @@
       <c r="H35" s="55"/>
       <c r="I35" s="54"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="59" t="s">
         <v>44</v>
       </c>
@@ -2033,7 +2064,7 @@
       <c r="H36" s="56"/>
       <c r="I36" s="57"/>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="59" t="s">
         <v>29</v>
       </c>
@@ -2041,7 +2072,7 @@
       <c r="D37" s="59"/>
       <c r="E37" s="59"/>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="59" t="s">
         <v>30</v>
       </c>
@@ -2049,13 +2080,13 @@
       <c r="D38" s="59"/>
       <c r="E38" s="59"/>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="59" t="s">
         <v>38</v>
       </c>
@@ -2063,7 +2094,7 @@
       <c r="D40" s="59"/>
       <c r="E40" s="59"/>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="60" t="s">
         <v>39</v>
       </c>
@@ -2073,7 +2104,7 @@
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="62" t="s">
         <v>41</v>
       </c>
@@ -2083,7 +2114,7 @@
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
     </row>
-    <row r="43" spans="2:9" ht="51">
+    <row r="43" spans="2:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B43" s="63" t="s">
         <v>43</v>
       </c>
@@ -2093,19 +2124,19 @@
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="59"/>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
       <c r="E44" s="59"/>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="59"/>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
       <c r="E45" s="59"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="59"/>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
@@ -2113,14 +2144,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2133,6 +2156,14 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Nils: Knoten-/DB-überprüfung geschrieben Modul Database: enthält nun Möglichkeit die Datenbank auf Verbindung der Knoten zu Testen. Bei Drücken auf Go wird vorhandene Datenbank getestet. Ausgabe etwaiger Fehler über Konsole. In äußerster for-Schleife der Testfunktion muss letzte eingetragene ID stehen.
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>Name </t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>GUI: Thomas und David, welche für das Graphical User Interface zuständig sind</t>
-  </si>
-  <si>
-    <t>noch unbestimmt (wird zeitnah geklärt, wer das machen soll)</t>
   </si>
   <si>
     <r>
@@ -336,9 +333,6 @@
   </si>
   <si>
     <t>Nils</t>
-  </si>
-  <si>
-    <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
   </si>
   <si>
     <t>A1: A2 aus Ziel 3 auf Basis von Erics ergebnissen
@@ -463,9 +457,58 @@
     </r>
   </si>
   <si>
-    <t>A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
-A2: Datenbank in UASJ-Maps bringen
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(z-koordinate &amp; Raumnummern fehlen noch)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Routenzeichnung schreiben</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Datenbank in UASJ-Maps bringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -476,7 +519,7 @@
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -649,6 +692,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF00B0F0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1098,6 +1146,51 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1107,15 +1200,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1124,42 +1208,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1533,7 +1581,7 @@
   <dimension ref="B2:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:H18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1565,7 +1613,7 @@
     </row>
     <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1622,11 +1670,11 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -1640,11 +1688,11 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1658,11 +1706,11 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,11 +1724,11 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="F9" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="47"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,11 +1742,11 @@
       <c r="E10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1712,11 +1760,11 @@
       <c r="E11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,11 +1774,11 @@
       <c r="E12" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,11 +1788,11 @@
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="74"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,11 +1839,11 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="71"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
@@ -1803,17 +1851,17 @@
         <v>6</v>
       </c>
       <c r="C17" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="49"/>
       <c r="E17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="F17" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="73"/>
+      <c r="H17" s="74"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
@@ -1821,17 +1869,17 @@
         <v>7</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18" s="49"/>
       <c r="E18" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="84" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="85"/>
-      <c r="H18" s="86"/>
+      <c r="F18" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
@@ -1839,17 +1887,17 @@
         <v>8</v>
       </c>
       <c r="C19" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="69" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="70"/>
-      <c r="H19" s="71"/>
+      <c r="F19" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="73"/>
+      <c r="H19" s="74"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
@@ -1857,35 +1905,35 @@
         <v>23</v>
       </c>
       <c r="C20" s="47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="70"/>
-      <c r="H20" s="71"/>
+      <c r="F20" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="73"/>
+      <c r="H20" s="74"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
       <c r="B21" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="51" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
+        <v>55</v>
+      </c>
+      <c r="F21" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="73"/>
+      <c r="H21" s="74"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -1897,31 +1945,31 @@
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
       <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="51" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>51</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="70"/>
-      <c r="H23" s="71"/>
+      <c r="F23" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1968,11 +2016,11 @@
       <c r="E26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
       <c r="I26" s="25"/>
     </row>
     <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1984,9 +2032,9 @@
       <c r="E27" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="81"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="83"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1998,9 +2046,9 @@
       <c r="E28" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,9 +2060,9 @@
       <c r="E29" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="77"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="68"/>
       <c r="I29" s="24"/>
     </row>
     <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2144,6 +2192,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2156,17 +2212,9 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Datum eingeben" prompt="Geben Sie das Datum für Montag dieser Woche ein. Das Enddatum wird automatisch angezeigt." sqref="F3:F4"/>
   </dataValidations>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
David: Test zu Wochenziel3 A3
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
+    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,28 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-ich weiß ja nicht wann du das letzte mal geschaut hast aber jetzt ist das bei set_floor implementiert (case 4 bis 8)</t>
+ich weiß ja nicht wann du das letzte mal geschaut hast aber jetzt ist das bei set_floor implementiert (case 4 bis 8)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">David:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>es geht um andere Funktionen, die zur Ausführung noch benötigt wurden. zudem ist mir aufgefallen, dass es an Ziel3 A1 von GO hängt, weil es ja an diese Lösung angepasst werden muss</t>
         </r>
       </text>
     </comment>
@@ -514,12 +535,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1146,6 +1167,33 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1164,15 +1212,6 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1190,24 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,7 +1313,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1366,7 +1387,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1401,7 +1421,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1577,27 +1596,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1611,7 +1630,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>60</v>
       </c>
@@ -1631,7 +1650,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1641,7 +1660,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="15.95" customHeight="1">
       <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1678,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="44" t="s">
         <v>5</v>
       </c>
@@ -1670,14 +1689,14 @@
       <c r="E6" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="22.5">
       <c r="B7" s="48" t="s">
         <v>6</v>
       </c>
@@ -1688,14 +1707,14 @@
       <c r="E7" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="60" customHeight="1">
       <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
@@ -1706,14 +1725,14 @@
       <c r="E8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="111" customHeight="1">
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1724,14 +1743,14 @@
       <c r="E9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="47"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
@@ -1742,14 +1761,14 @@
       <c r="E10" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1">
       <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
@@ -1760,42 +1779,42 @@
       <c r="E11" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1">
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
       <c r="D12" s="26"/>
       <c r="E12" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="39" customHeight="1">
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
       <c r="D13" s="26"/>
       <c r="E13" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="72" t="s">
+      <c r="F13" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="73"/>
-      <c r="H13" s="74"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="71"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="26"/>
@@ -1805,7 +1824,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="39" t="s">
         <v>3</v>
       </c>
@@ -1828,7 +1847,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="44" t="s">
         <v>5</v>
       </c>
@@ -1839,14 +1858,14 @@
       <c r="E16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="101.25">
       <c r="B17" s="48" t="s">
         <v>6</v>
       </c>
@@ -1857,14 +1876,14 @@
       <c r="E17" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="72" t="s">
+      <c r="F17" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="74"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="144" customHeight="1">
       <c r="B18" s="48" t="s">
         <v>7</v>
       </c>
@@ -1875,14 +1894,14 @@
       <c r="E18" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F18" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="45">
       <c r="B19" s="48" t="s">
         <v>8</v>
       </c>
@@ -1893,14 +1912,14 @@
       <c r="E19" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="101.25">
       <c r="B20" s="48" t="s">
         <v>23</v>
       </c>
@@ -1911,14 +1930,14 @@
       <c r="E20" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="72" t="s">
+      <c r="F20" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="73"/>
-      <c r="H20" s="74"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="40.799999999999997" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="45">
       <c r="B21" s="58" t="s">
         <v>55</v>
       </c>
@@ -1929,14 +1948,14 @@
       <c r="E21" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="72" t="s">
+      <c r="F21" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="74"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="48" t="s">
         <v>36</v>
       </c>
@@ -1947,14 +1966,14 @@
       <c r="E22" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="68.25" customHeight="1">
       <c r="B23" s="48" t="s">
         <v>49</v>
       </c>
@@ -1965,14 +1984,14 @@
       <c r="E23" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="72" t="s">
+      <c r="F23" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="26"/>
@@ -1982,7 +2001,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B25" s="39" t="s">
         <v>3</v>
       </c>
@@ -2005,7 +2024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B26" s="44" t="s">
         <v>5</v>
       </c>
@@ -2016,14 +2035,14 @@
       <c r="E26" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B27" s="48" t="s">
         <v>6</v>
       </c>
@@ -2032,12 +2051,12 @@
       <c r="E27" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B28" s="48" t="s">
         <v>7</v>
       </c>
@@ -2046,12 +2065,12 @@
       <c r="E28" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B29" s="48" t="s">
         <v>8</v>
       </c>
@@ -2060,21 +2079,21 @@
       <c r="E29" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="68"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="77"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="59" t="s">
         <v>27</v>
       </c>
@@ -2082,7 +2101,7 @@
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
     </row>
-    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B34" s="59" t="s">
         <v>47</v>
       </c>
@@ -2092,7 +2111,7 @@
       <c r="H34" s="53"/>
       <c r="I34" s="54"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="59" t="s">
         <v>28</v>
       </c>
@@ -2102,7 +2121,7 @@
       <c r="H35" s="55"/>
       <c r="I35" s="54"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="59" t="s">
         <v>44</v>
       </c>
@@ -2112,7 +2131,7 @@
       <c r="H36" s="56"/>
       <c r="I36" s="57"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="59" t="s">
         <v>29</v>
       </c>
@@ -2120,7 +2139,7 @@
       <c r="D37" s="59"/>
       <c r="E37" s="59"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="59" t="s">
         <v>30</v>
       </c>
@@ -2128,13 +2147,13 @@
       <c r="D38" s="59"/>
       <c r="E38" s="59"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="59"/>
       <c r="C39" s="59"/>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="59" t="s">
         <v>38</v>
       </c>
@@ -2142,7 +2161,7 @@
       <c r="D40" s="59"/>
       <c r="E40" s="59"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="60" t="s">
         <v>39</v>
       </c>
@@ -2152,7 +2171,7 @@
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="62" t="s">
         <v>41</v>
       </c>
@@ -2162,7 +2181,7 @@
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
     </row>
-    <row r="43" spans="2:9" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="51">
       <c r="B43" s="63" t="s">
         <v>43</v>
       </c>
@@ -2172,19 +2191,19 @@
       <c r="D43" s="59"/>
       <c r="E43" s="59"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="59"/>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
       <c r="E44" s="59"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="B45" s="59"/>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
       <c r="E45" s="59"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9">
       <c r="B46" s="59"/>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
@@ -2192,14 +2211,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2212,6 +2223,14 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
Laura: - Database.csv aktualisiert - Wochenziele aktualieisert
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Wochenpläne!$A$1:$H$35</definedName>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Name </t>
   </si>
@@ -265,10 +266,12 @@
     <t>GUI: Thomas und David, welche für das Graphical User Interface zuständig sind</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)
-</t>
-    </r>
+    <t>Laura &amp; Nils</t>
+  </si>
+  <si>
+    <t>Sind am 3. Januar durch die Häuser 1, 2, 3 und 5 gelaufen um Knotensetzung darauf zu überprüfen, ob sie sinnvoll ist und um mögliche Sackgassen zu finden oder unerwartete Durchgänge</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -276,7 +279,42 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)</t>
+      <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
+    </r>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>A1: csv dateien für Haus 1, 2 und 3 anlegen (Knoten eintragen)</t>
+  </si>
+  <si>
+    <t>A1: Modultests duchführen</t>
+  </si>
+  <si>
+    <t>Nils</t>
+  </si>
+  <si>
+    <t>Plan der Wochenziele</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)</t>
     </r>
     <r>
       <rPr>
@@ -291,11 +329,11 @@
     <r>
       <rPr>
         <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?</t>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)</t>
     </r>
     <r>
       <rPr>
@@ -310,6 +348,25 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
         <color rgb="FF00B050"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -318,12 +375,6 @@
     </r>
   </si>
   <si>
-    <t>Laura &amp; Nils</t>
-  </si>
-  <si>
-    <t>Sind am 3. Januar durch die Häuser 1, 2, 3 und 5 gelaufen um Knotensetzung darauf zu überprüfen, ob sie sinnvoll ist und um mögliche Sackgassen zu finden oder unerwartete Durchgänge</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -331,7 +382,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten</t>
+      <t>A1: Problem Singeltouch lösen</t>
     </r>
     <r>
       <rPr>
@@ -340,26 +391,9 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
-    </r>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>A1: csv dateien für Haus 1, 2 und 3 anlegen (Knoten eintragen)</t>
-  </si>
-  <si>
-    <t>A1: Modultests duchführen</t>
-  </si>
-  <si>
-    <t>Nils</t>
-  </si>
-  <si>
-    <t>A1: A2 aus Ziel 3 auf Basis von Erics ergebnissen
-A2: Absprache mit Team GUI zwecks Farbe und Form Buttons</t>
-  </si>
-  <si>
+      <t xml:space="preserve">
+A2: </t>
+    </r>
     <r>
       <rPr>
         <sz val="8"/>
@@ -367,6 +401,114 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">Ebenen von Haus 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">und einem weiteren Haus grafisch darstellen
+A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric - wird auf Ziel 4 verschoben, da ich es sinnvoller finde, mich dem anzupassen, was Eric schon gemacht hat, als erstmal parallel was neues zu erfinden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Startbildschirm entwerfen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt</t>
     </r>
     <r>
@@ -377,20 +519,123 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-A2: Erstellung Testprotokoll für Pathfinding
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Erstellung Testprotokoll für Pathfinding
 A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
     </r>
   </si>
   <si>
-    <t>A1: siehe A2:Ziel4:GD</t>
+    <t>A1:Campus zeichnen
+A2: Textausgabe</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Datenbank in UASJ-Maps bringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: Rückgabewerte für GUI Ziel4 A4 einbauen
+A5: Haus 1,2,3 zusammenhängend zeichnen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: siehe A2:Ziel4:GD - verschoben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A2: Single- und Multitouch in UASJ-Maps einbringen
+A3: Besprochene Lösung für Eingabe Routing und LuL
+A4: Textfeld für Haus und Ebene oben links einfügen</t>
+    </r>
   </si>
   <si>
     <t>A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
 A2: Architekturmodell finden
-A3: GUI auf den neuesten Stand bringen</t>
-  </si>
-  <si>
-    <t>Plan der Wochenziele</t>
+A3: UML auf den neuesten Stand bringen</t>
+  </si>
+  <si>
+    <t>A1: Integrationstest durchführen</t>
+  </si>
+  <si>
+    <t>A1: Alle Tests an Endversion durchführen und protokollieren</t>
+  </si>
+  <si>
+    <t>A1: Logo und Startupscreen reinbringen
+A2: ausgegraute Buttons 
+A3: Optionenmenü umsetzen
+A4: Initialzoom in Go-Button implementieren</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: A2 aus Ziel 3 auf Basis von Erics ergebnissen
+A2: Absprache mit Team GUI zwecks Farbe und Form Buttons
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Startupscreen an Jan und Marcus schicken und um Meinung fragen</t>
+    </r>
   </si>
   <si>
     <r>
@@ -400,136 +645,31 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Raumnummern fehlen noch)
 </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric - wird auf Ziel 4 verschoben, da ich es sinnvoller finde, mich dem anzupassen, was Eric schon gemacht hat, als erstmal parallel was neues zu erfinden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A3: Startbildschirm entwerfen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1: Problem Singeltouch lösen
-A2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ebenen von Haus 5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">und einem weiteren Haus grafisch darstellen
-A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(z-koordinate &amp; Raumnummern fehlen noch)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Routenzeichnung schreiben</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Datenbank in UASJ-Maps bringen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht</t>
-    </r>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Routenzeichnung schreiben
+A3: Campus in csv datei eintragen</t>
+    </r>
+  </si>
+  <si>
+    <t>A1: Entwurf Präsentation</t>
   </si>
 </sst>
 </file>
@@ -718,6 +858,7 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1101,10 +1242,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1132,10 +1269,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1167,6 +1300,59 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1176,15 +1362,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,42 +1370,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1599,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1632,7 +1773,7 @@
     </row>
     <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1661,162 +1802,162 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:14" ht="15.95" customHeight="1">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="45">
         <v>40899</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="46">
+      <c r="F5" s="45">
         <v>40906</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="21"/>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="74"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="22.5">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="48" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="48" t="s">
+      <c r="D8" s="63"/>
+      <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="48" t="s">
+      <c r="D9" s="63"/>
+      <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="47"/>
+      <c r="F9" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="49" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="26"/>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="49" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="26"/>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1">
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1">
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="26"/>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="83"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
       <c r="F14" s="24"/>
@@ -1825,170 +1966,170 @@
       <c r="I14" s="24"/>
     </row>
     <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="46">
+      <c r="C15" s="45">
         <v>40913</v>
       </c>
       <c r="D15" s="30"/>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="46">
+      <c r="F15" s="45">
         <v>40920</v>
       </c>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="43"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="31"/>
       <c r="L15" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="32"/>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="71"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="101.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="73"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="2:12" ht="144" customHeight="1">
+      <c r="B18" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="2:12" ht="45">
+      <c r="B19" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="73"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="2:12" ht="101.25">
+      <c r="B20" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="83"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="2:12" ht="57.75" customHeight="1">
+      <c r="B21" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="48"/>
+      <c r="E21" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="73"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" ht="22.5">
+      <c r="B22" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="48"/>
+      <c r="E22" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="73"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="2:12" ht="68.25" customHeight="1">
+      <c r="B23" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="2:12" ht="144" customHeight="1">
-      <c r="B18" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="49"/>
-      <c r="E18" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="2:12" ht="45">
-      <c r="B19" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="48" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="70"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="24"/>
-    </row>
-    <row r="20" spans="2:12" ht="101.25">
-      <c r="B20" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="70"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="24"/>
-    </row>
-    <row r="21" spans="2:12" ht="45">
-      <c r="B21" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="69" t="s">
+      <c r="C23" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="24"/>
-    </row>
-    <row r="22" spans="2:12" ht="22.5">
-      <c r="B22" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="24"/>
-    </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1">
-      <c r="B23" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="49"/>
-      <c r="E23" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="69" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="70"/>
-      <c r="H23" s="71"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -2002,90 +2143,103 @@
       <c r="I24" s="33"/>
     </row>
     <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25" s="45">
         <v>40927</v>
       </c>
       <c r="D25" s="30"/>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="46">
+      <c r="F25" s="45">
         <v>40934</v>
       </c>
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="43"/>
+      <c r="H25" s="42"/>
       <c r="I25" s="31"/>
       <c r="L25" s="29" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="44" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="32"/>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="17.100000000000001" customHeight="1">
-      <c r="B27" s="48" t="s">
+    <row r="27" spans="2:12" ht="45.75">
+      <c r="B27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="38"/>
+      <c r="C27" s="64" t="s">
+        <v>66</v>
+      </c>
       <c r="D27" s="23"/>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="86"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="17.100000000000001" customHeight="1">
-      <c r="B28" s="48" t="s">
+    <row r="28" spans="2:12" ht="23.25">
+      <c r="B28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="65" t="s">
+        <v>60</v>
+      </c>
       <c r="D28" s="23"/>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="17.100000000000001" customHeight="1">
-      <c r="B29" s="48" t="s">
+    <row r="29" spans="2:12" ht="21.75" customHeight="1">
+      <c r="B29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="37" t="s">
+        <v>64</v>
+      </c>
       <c r="D29" s="23"/>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="77"/>
+      <c r="F29" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="73"/>
+      <c r="H29" s="74"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="17.100000000000001" customHeight="1">
-      <c r="B30" s="24"/>
+    <row r="30" spans="2:12">
+      <c r="B30" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="24"/>
@@ -2094,123 +2248,131 @@
       <c r="B32" s="24"/>
     </row>
     <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="57"/>
     </row>
     <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="54"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="52"/>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="54"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="H35" s="53"/>
     </row>
     <row r="36" spans="2:9">
-      <c r="B36" s="59" t="s">
+      <c r="B36" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="52"/>
     </row>
     <row r="37" spans="2:9">
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="I37" s="55"/>
     </row>
     <row r="38" spans="2:9">
-      <c r="B38" s="59" t="s">
+      <c r="B38" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
     </row>
     <row r="39" spans="2:9">
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
     </row>
     <row r="40" spans="2:9">
-      <c r="B40" s="59" t="s">
+      <c r="B40" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="59"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
     </row>
     <row r="41" spans="2:9">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
     </row>
     <row r="42" spans="2:9">
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
     </row>
     <row r="43" spans="2:9" ht="51">
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="64" t="s">
+      <c r="C43" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
     </row>
     <row r="44" spans="2:9">
-      <c r="B44" s="59"/>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="57"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
     </row>
     <row r="45" spans="2:9">
-      <c r="B45" s="59"/>
-      <c r="C45" s="59"/>
-      <c r="D45" s="59"/>
-      <c r="E45" s="59"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
     </row>
     <row r="46" spans="2:9">
-      <c r="B46" s="59"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2223,22 +2385,28 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" promptTitle="Datum eingeben" prompt="Geben Sie das Datum für Montag dieser Woche ein. Das Enddatum wird automatisch angezeigt." sqref="F3:F4"/>
   </dataValidations>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
David: Wochenziel abgehackt. TODO beim RoomSpinner: UML erweitern, Kommentare schreiben
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -582,29 +582,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: siehe A2:Ziel4:GD - verschoben</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A2: Single- und Multitouch in UASJ-Maps einbringen
-A3: Besprochene Lösung für Eingabe Routing und LuL
-A4: Textfeld für Haus und Ebene oben links einfügen</t>
-    </r>
-  </si>
-  <si>
     <t>A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
 A2: Architekturmodell finden
 A3: UML auf den neuesten Stand bringen</t>
@@ -670,6 +647,47 @@
   </si>
   <si>
     <t>A1: Entwurf Präsentation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: siehe A2:Ziel4:GD - verschoben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A2: Single- und Multitouch in UASJ-Maps einbringen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Besprochene Lösung für Eingabe Routing und LuL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A4: Textfeld für Haus und Ebene oben links einfügen</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1308,6 +1326,33 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1326,15 +1371,6 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1352,24 +1388,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1740,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -1830,11 +1848,11 @@
       <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="22.5">
@@ -1848,11 +1866,11 @@
       <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1">
@@ -1866,11 +1884,11 @@
       <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1">
@@ -1884,11 +1902,11 @@
       <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="73"/>
-      <c r="H9" s="74"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
       <c r="I9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1">
@@ -1902,11 +1920,11 @@
       <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1">
@@ -1920,11 +1938,11 @@
       <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1">
@@ -1934,11 +1952,11 @@
       <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1">
@@ -1948,11 +1966,11 @@
       <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
@@ -1999,11 +2017,11 @@
       <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="69" t="s">
+      <c r="F16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="70"/>
-      <c r="H16" s="71"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="101.25">
@@ -2017,11 +2035,11 @@
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="74"/>
+      <c r="F17" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="144" customHeight="1">
@@ -2035,11 +2053,11 @@
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F18" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="45">
@@ -2053,11 +2071,11 @@
       <c r="E19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="72" t="s">
+      <c r="F19" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="73"/>
-      <c r="H19" s="74"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="101.25">
@@ -2071,11 +2089,11 @@
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="83"/>
+      <c r="F20" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="67"/>
+      <c r="H20" s="68"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:12" ht="57.75" customHeight="1">
@@ -2089,11 +2107,11 @@
       <c r="E21" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="73"/>
-      <c r="H21" s="74"/>
+      <c r="F21" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:12" ht="22.5">
@@ -2107,11 +2125,11 @@
       <c r="E22" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="72" t="s">
+      <c r="F22" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="73"/>
-      <c r="H22" s="74"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:12" ht="68.25" customHeight="1">
@@ -2125,11 +2143,11 @@
       <c r="E23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="73"/>
-      <c r="H23" s="74"/>
+      <c r="F23" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -2176,11 +2194,11 @@
       <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="25"/>
     </row>
     <row r="27" spans="2:12" ht="45.75">
@@ -2188,15 +2206,15 @@
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="23.25">
@@ -2210,9 +2228,9 @@
       <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="21.75" customHeight="1">
@@ -2220,17 +2238,17 @@
         <v>8</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
+      <c r="F29" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
       <c r="I29" s="24"/>
     </row>
     <row r="30" spans="2:12">
@@ -2238,7 +2256,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
@@ -2365,14 +2383,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2385,6 +2395,14 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
Nils: GO: - Routenzeichnung/Positionszeichnung hinzugefügt - Getter für aktuelle Haus und Ebenenbezeichnung geschrieben PF: - Routenfindung an Übergabe eines Strings angepasst GUI: - kleine Änderung damit Änderung in ersten beiden Klassen keine Fehler hervorruft
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
+    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -295,9 +295,6 @@
     <t>Laura</t>
   </si>
   <si>
-    <t>A1: csv dateien für Haus 1, 2 und 3 anlegen (Knoten eintragen)</t>
-  </si>
-  <si>
     <t>A1: Modultests duchführen</t>
   </si>
   <si>
@@ -535,51 +532,6 @@
   <si>
     <t>A1:Campus zeichnen
 A2: Textausgabe</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Datenbank in UASJ-Maps bringen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A4: Rückgabewerte für GUI Ziel4 A4 einbauen
-A5: Haus 1,2,3 zusammenhängend zeichnen</t>
-    </r>
   </si>
   <si>
     <t>A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
@@ -615,37 +567,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Raumnummern fehlen noch)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Routenzeichnung schreiben
-A3: Campus in csv datei eintragen</t>
-    </r>
-  </si>
-  <si>
     <t>A1: Entwurf Präsentation</t>
   </si>
   <si>
@@ -687,18 +608,126 @@
       </rPr>
       <t xml:space="preserve">
 A4: Textfeld für Haus und Ebene oben links einfügen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Raumnummern fehlen noch)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Routenzeichnung schreiben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A3: Campus in csv datei eintragen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Datenbank in UASJ-Maps bringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht
+A4: Rückgabewerte für GUI Ziel4 A4 einbauen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A5: Haus 1,2,3 zusammenhängend zeichnen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: csv dateien für Haus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1, 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> und 3 anlegen (Knoten eintragen)</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1326,6 +1355,51 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1343,51 +1417,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1472,7 +1501,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1546,6 +1575,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1580,6 +1610,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1755,27 +1786,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1789,9 +1820,9 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1">
+    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1809,7 +1840,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1819,7 +1850,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1868,7 @@
       <c r="H5" s="40"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
@@ -1848,14 +1879,14 @@
       <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="71"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="22.5">
+    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
@@ -1866,14 +1897,14 @@
       <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
         <v>7</v>
       </c>
@@ -1884,14 +1915,14 @@
       <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
         <v>8</v>
       </c>
@@ -1902,14 +1933,14 @@
       <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
+      <c r="F9" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="46"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
@@ -1920,14 +1951,14 @@
       <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
@@ -1938,42 +1969,42 @@
       <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="26"/>
       <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="26"/>
       <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="83"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="26"/>
@@ -1983,7 +2014,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="38" t="s">
         <v>3</v>
       </c>
@@ -2006,7 +2037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
         <v>5</v>
       </c>
@@ -2017,50 +2048,50 @@
       <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="101.25">
+    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="B17" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
+      <c r="F17" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="144" customHeight="1">
+    <row r="18" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83"/>
+      <c r="F18" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="45">
+    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="47" t="s">
         <v>8</v>
       </c>
@@ -2071,50 +2102,50 @@
       <c r="E19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="74" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="F19" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="101.25">
+    <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
+      <c r="F20" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="83"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="57.75" customHeight="1">
+    <row r="21" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="48"/>
       <c r="E21" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="73"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="22.5">
+    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
         <v>36</v>
       </c>
@@ -2125,14 +2156,14 @@
       <c r="E22" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="73"/>
+      <c r="F22" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1">
+    <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
         <v>48</v>
       </c>
@@ -2143,14 +2174,14 @@
       <c r="E23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="74" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="73"/>
+      <c r="F23" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="26"/>
@@ -2160,7 +2191,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="38" t="s">
         <v>3</v>
       </c>
@@ -2183,7 +2214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="43" t="s">
         <v>5</v>
       </c>
@@ -2194,78 +2225,78 @@
       <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="45.75">
+    <row r="27" spans="2:12" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B27" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="86"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="23.25">
+    <row r="28" spans="2:12" ht="21" x14ac:dyDescent="0.25">
       <c r="B28" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="21.75" customHeight="1">
+    <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
+      <c r="F29" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="56" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="57" t="s">
         <v>27</v>
       </c>
@@ -2273,7 +2304,7 @@
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
     </row>
-    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="57" t="s">
         <v>47</v>
       </c>
@@ -2283,7 +2314,7 @@
       <c r="H34" s="51"/>
       <c r="I34" s="52"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="57" t="s">
         <v>28</v>
       </c>
@@ -2292,7 +2323,7 @@
       <c r="E35" s="57"/>
       <c r="H35" s="53"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="57" t="s">
         <v>44</v>
       </c>
@@ -2302,7 +2333,7 @@
       <c r="H36" s="54"/>
       <c r="I36" s="52"/>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="57" t="s">
         <v>29</v>
       </c>
@@ -2311,7 +2342,7 @@
       <c r="E37" s="57"/>
       <c r="I37" s="55"/>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="57" t="s">
         <v>30</v>
       </c>
@@ -2319,13 +2350,13 @@
       <c r="D38" s="57"/>
       <c r="E38" s="57"/>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
       <c r="E39" s="57"/>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="57" t="s">
         <v>38</v>
       </c>
@@ -2333,7 +2364,7 @@
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="58" t="s">
         <v>39</v>
       </c>
@@ -2343,7 +2374,7 @@
       <c r="D41" s="57"/>
       <c r="E41" s="57"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="60" t="s">
         <v>41</v>
       </c>
@@ -2353,7 +2384,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="2:9" ht="51">
+    <row r="43" spans="2:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B43" s="61" t="s">
         <v>43</v>
       </c>
@@ -2363,19 +2394,19 @@
       <c r="D43" s="57"/>
       <c r="E43" s="57"/>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
       <c r="D44" s="57"/>
       <c r="E44" s="57"/>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
       <c r="D45" s="57"/>
       <c r="E45" s="57"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
       <c r="D46" s="57"/>
@@ -2383,6 +2414,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2395,14 +2434,6 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -2416,14 +2447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nils: GO: - Textausgabe implementiert - kleine Änderung in Funktionen der Ebenen/Hausnummernausgabe
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -530,10 +530,6 @@
     </r>
   </si>
   <si>
-    <t>A1:Campus zeichnen
-A2: Textausgabe</t>
-  </si>
-  <si>
     <t>A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
 A2: Architekturmodell finden
 A3: UML auf den neuesten Stand bringen</t>
@@ -716,6 +712,21 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> und 3 anlegen (Knoten eintragen)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1:Campus zeichnen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Textausgabe</t>
     </r>
   </si>
 </sst>
@@ -1355,6 +1366,33 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1364,15 +1402,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1399,24 +1428,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1789,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1879,11 +1890,11 @@
       <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -1897,11 +1908,11 @@
       <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,11 +1926,11 @@
       <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -1933,11 +1944,11 @@
       <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
       <c r="I9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1951,11 +1962,11 @@
       <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,11 +1980,11 @@
       <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,11 +1994,11 @@
       <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1997,11 +2008,11 @@
       <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2048,11 +2059,11 @@
       <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="72" t="s">
+      <c r="F16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="73"/>
-      <c r="H16" s="74"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
@@ -2066,11 +2077,11 @@
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="F17" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="144" customHeight="1" x14ac:dyDescent="0.25">
@@ -2084,11 +2095,11 @@
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
+      <c r="F18" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
@@ -2102,11 +2113,11 @@
       <c r="E19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="69" t="s">
+      <c r="F19" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="70"/>
-      <c r="H19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
@@ -2120,11 +2131,11 @@
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="83"/>
+      <c r="F20" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="67"/>
+      <c r="H20" s="68"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,11 +2149,11 @@
       <c r="E21" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
+      <c r="F21" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -2156,11 +2167,11 @@
       <c r="E22" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="F22" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2174,11 +2185,11 @@
       <c r="E23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" s="70"/>
-      <c r="H23" s="71"/>
+      <c r="F23" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2225,11 +2236,11 @@
       <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="73"/>
-      <c r="H26" s="74"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="25"/>
     </row>
     <row r="27" spans="2:12" ht="41.4" x14ac:dyDescent="0.25">
@@ -2237,15 +2248,15 @@
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="21" x14ac:dyDescent="0.25">
@@ -2253,15 +2264,15 @@
         <v>7</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,17 +2280,17 @@
         <v>8</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="70"/>
-      <c r="H29" s="71"/>
+      <c r="F29" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
       <c r="I29" s="24"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -2287,7 +2298,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2414,14 +2425,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2434,6 +2437,14 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
David: nach SWT viele Änderungen, logo, DB, campus, multi_touch, ...
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -668,21 +668,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">A1:Campus zeichnen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Textausgabe</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <sz val="8"/>
         <color rgb="FF00B050"/>
@@ -753,6 +738,30 @@
 A3: Optionenmenü umsetzen
 A4: Initialzoom in Go-Button implementieren
 A5: David: Test: Sind Räume von RommSpinner auch alle in Datenbank?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1:Campus zeichnen
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A2: Textausgabe
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Funktion für Übergabewerte von Haus und Ebene wegen offset überprüfen</t>
     </r>
   </si>
 </sst>
@@ -764,7 +773,7 @@
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -943,6 +952,11 @@
     <font>
       <sz val="8"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1825,7 +1839,7 @@
   <dimension ref="B2:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
@@ -2102,7 +2116,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G17" s="70"/>
       <c r="H17" s="71"/>
@@ -2272,7 +2286,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
@@ -2283,12 +2297,12 @@
       <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="23.25">
+    <row r="28" spans="2:12" ht="45.75">
       <c r="B28" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="47" t="s">

</xml_diff>

<commit_message>
Nils: GO: -Fehlerhafte Funktionen korrgiert GUI: - an Änderungen (s.o.) angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
+    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -560,46 +560,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(Raumnummern fehlen noch)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Routenzeichnung schreiben</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A3: Campus in csv datei eintragen</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
 </t>
     </r>
@@ -742,6 +702,46 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Routenzeichnung schreiben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A3: Campus in csv datei eintragen</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">A1:Campus zeichnen
 </t>
     </r>
@@ -752,28 +752,20 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">A2: Textausgabe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: Funktion für Übergabewerte von Haus und Ebene wegen offset überprüfen</t>
+      <t>A2: Textausgabe
+A3: Funktion für Übergabewerte von Haus und Ebene wegen offset überprüfen</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -952,11 +944,6 @@
     <font>
       <sz val="8"/>
       <color theme="1" tint="0.34998626667073579"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1406,6 +1393,33 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1415,15 +1429,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1450,24 +1455,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1552,7 +1539,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1626,6 +1613,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1660,6 +1648,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1835,27 +1824,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +1858,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1">
+    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>54</v>
       </c>
@@ -1889,7 +1878,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1899,7 +1888,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.95" customHeight="1">
+    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
@@ -1917,7 +1906,7 @@
       <c r="H5" s="40"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
@@ -1928,14 +1917,14 @@
       <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="84" t="s">
+      <c r="F6" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="22.5">
+    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
@@ -1946,14 +1935,14 @@
       <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="81" t="s">
+      <c r="F7" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="82"/>
-      <c r="H7" s="83"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="68"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1">
+    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
         <v>7</v>
       </c>
@@ -1964,14 +1953,14 @@
       <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="70"/>
-      <c r="H8" s="71"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="73"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1">
+    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
         <v>8</v>
       </c>
@@ -1982,14 +1971,14 @@
       <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="71"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="73"/>
       <c r="I9" s="46"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1">
+    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
@@ -2000,14 +1989,14 @@
       <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="83"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
@@ -2018,42 +2007,42 @@
       <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="81" t="s">
+      <c r="F11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="82"/>
-      <c r="H11" s="83"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="26"/>
       <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="82"/>
-      <c r="H12" s="83"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1">
+    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="26"/>
       <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="26"/>
@@ -2063,7 +2052,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="38" t="s">
         <v>3</v>
       </c>
@@ -2086,7 +2075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
         <v>5</v>
       </c>
@@ -2097,14 +2086,14 @@
       <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="72" t="s">
+      <c r="F16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="73"/>
-      <c r="H16" s="74"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="80"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="101.25">
+    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
       <c r="B17" s="47" t="s">
         <v>6</v>
       </c>
@@ -2115,14 +2104,14 @@
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="F17" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="72"/>
+      <c r="H17" s="73"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="144" customHeight="1">
+    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
       <c r="B18" s="47" t="s">
         <v>7</v>
       </c>
@@ -2133,14 +2122,14 @@
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="76"/>
-      <c r="H18" s="77"/>
+      <c r="F18" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="82"/>
+      <c r="H18" s="83"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="45">
+    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="47" t="s">
         <v>8</v>
       </c>
@@ -2151,14 +2140,14 @@
       <c r="E19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="69" t="s">
+      <c r="F19" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="70"/>
-      <c r="H19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="73"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="101.25">
+    <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>23</v>
       </c>
@@ -2169,14 +2158,14 @@
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="82"/>
-      <c r="H20" s="83"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="68"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="57.75" customHeight="1">
+    <row r="21" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="56" t="s">
         <v>53</v>
       </c>
@@ -2187,14 +2176,14 @@
       <c r="E21" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
+      <c r="F21" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="72"/>
+      <c r="H21" s="73"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="22.5">
+    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
         <v>36</v>
       </c>
@@ -2205,14 +2194,14 @@
       <c r="E22" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="F22" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1">
+    <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
         <v>48</v>
       </c>
@@ -2223,14 +2212,14 @@
       <c r="E23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="69" t="s">
+      <c r="F23" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="70"/>
-      <c r="H23" s="71"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="73"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="26"/>
@@ -2240,7 +2229,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
+    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="38" t="s">
         <v>3</v>
       </c>
@@ -2263,7 +2252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="43" t="s">
         <v>5</v>
       </c>
@@ -2274,30 +2263,30 @@
       <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="72" t="s">
+      <c r="F26" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="73"/>
-      <c r="H26" s="74"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="80"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="68.25">
+    <row r="27" spans="2:12" ht="61.8" x14ac:dyDescent="0.25">
       <c r="B27" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="78"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="80"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="86"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="45.75">
+    <row r="28" spans="2:12" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B28" s="47" t="s">
         <v>7</v>
       </c>
@@ -2308,12 +2297,12 @@
       <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="68"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="21.75" customHeight="1">
+    <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="47" t="s">
         <v>8</v>
       </c>
@@ -2324,14 +2313,14 @@
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="69" t="s">
+      <c r="F29" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="70"/>
-      <c r="H29" s="71"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="73"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="56" t="s">
         <v>22</v>
       </c>
@@ -2339,13 +2328,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="57" t="s">
         <v>27</v>
       </c>
@@ -2353,7 +2342,7 @@
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
     </row>
-    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="57" t="s">
         <v>47</v>
       </c>
@@ -2363,7 +2352,7 @@
       <c r="H34" s="51"/>
       <c r="I34" s="52"/>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="57" t="s">
         <v>28</v>
       </c>
@@ -2372,7 +2361,7 @@
       <c r="E35" s="57"/>
       <c r="H35" s="53"/>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="57" t="s">
         <v>44</v>
       </c>
@@ -2382,7 +2371,7 @@
       <c r="H36" s="54"/>
       <c r="I36" s="52"/>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="57" t="s">
         <v>29</v>
       </c>
@@ -2391,7 +2380,7 @@
       <c r="E37" s="57"/>
       <c r="I37" s="55"/>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="57" t="s">
         <v>30</v>
       </c>
@@ -2399,13 +2388,13 @@
       <c r="D38" s="57"/>
       <c r="E38" s="57"/>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
       <c r="E39" s="57"/>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="57" t="s">
         <v>38</v>
       </c>
@@ -2413,7 +2402,7 @@
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="58" t="s">
         <v>39</v>
       </c>
@@ -2423,7 +2412,7 @@
       <c r="D41" s="57"/>
       <c r="E41" s="57"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="60" t="s">
         <v>41</v>
       </c>
@@ -2433,7 +2422,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="2:9" ht="51">
+    <row r="43" spans="2:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B43" s="61" t="s">
         <v>43</v>
       </c>
@@ -2443,19 +2432,19 @@
       <c r="D43" s="57"/>
       <c r="E43" s="57"/>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
       <c r="D44" s="57"/>
       <c r="E44" s="57"/>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
       <c r="D45" s="57"/>
       <c r="E45" s="57"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
       <c r="D46" s="57"/>
@@ -2463,14 +2452,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2483,6 +2464,14 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
Laura/Nils: Plan der Wochenziele angepasst
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -271,26 +271,6 @@
     <t>Sind am 3. Januar durch die Häuser 1, 2, 3 und 5 gelaufen um Knotensetzung darauf zu überprüfen, ob sie sinnvoll ist und um mögliche Sackgassen zu finden oder unerwartete Durchgänge</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
-    </r>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
@@ -378,36 +358,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A1: Problem Singeltouch lösen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A2: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ebenen von Haus 5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">und einem weiteren Haus grafisch darstellen
-A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) </t>
+      <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt</t>
     </r>
     <r>
       <rPr>
@@ -426,112 +377,9 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric - wird auf Ziel 4 verschoben, da ich es sinnvoller finde, mich dem anzupassen, was Eric schon gemacht hat, als erstmal parallel was neues zu erfinden</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: Startbildschirm entwerfen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>A2: Erstellung Testprotokoll für Pathfinding
 A3: Erstellung Testprogramm Pathfinding (eventuell automatische Tests, die direkt ins Testprotokoll schreiben)</t>
     </r>
-  </si>
-  <si>
-    <t>A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
-A2: Architekturmodell finden
-A3: UML auf den neuesten Stand bringen</t>
   </si>
   <si>
     <t>A1: Integrationstest durchführen</t>
@@ -557,124 +405,6 @@
   </si>
   <si>
     <t>A1: Entwurf Präsentation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Datenbank in UASJ-Maps bringen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht
-A4: Rückgabewerte für GUI Ziel4 A4 einbauen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A5: Haus 1,2,3 zusammenhängend zeichnen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1: csv dateien für Haus </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>1, 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> und 3 anlegen (Knoten eintragen)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A1: siehe A2:Ziel4:GD - verschoben</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A2: Single- und Multitouch in UASJ-Maps einbringen
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: Besprochene Lösung für Eingabe Routing und LuL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A4: Textfeld für Haus und Ebene oben links einfügen</t>
-    </r>
   </si>
   <si>
     <r>
@@ -742,7 +472,238 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">A1:Campus zeichnen
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Problem Singeltouch lösen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A2: Ebenen von Haus 5 und einem weiteren Haus grafisch darstellen
+A3: Campus grafisch Darstellen mit ergebnissen von David (Ziel2, GUI, A1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: in der setFloor() restliche freie Navi umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A5: überlegen ob Zeichnen von Ebene und Position mit gleicher funktion (z.B. drawRouteOrPosition() ) geschehen soll, nach Davids Vorschlag Die Route mit einem Symbol (z.B. Kreuz) anfangen und enden zu lassen - Absprache mit Laura bitte</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Haus 5 testen mit Pathfinding und grafischer Ausgabe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Datenbank in UASJ-Maps bringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Mit GUI ausmachen, wer Datenbankzugriff bei Raumsuche/Start/Ziel macht
+A4: Rückgabewerte für GUI Ziel4 A4 einbauen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A5: Haus 1,2,3 zusammenhängend zeichnen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: siehe A2:Ziel4:GD - verschoben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Single- und Multitouch in UASJ-Maps einbringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Besprochene Lösung für Eingabe Routing und LuL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: Textfeld für Haus und Ebene oben links einfügen</t>
+    </r>
+  </si>
+  <si>
+    <t>A1: csv dateien für Haus 1, 2 und 3 anlegen (Knoten eintragen)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A1: Benutzerhandbuch erstellen (erstmal mit Bildern aus dem Pflichtenheft, die später mit Bildschirmfotos vom programm ersetzt werden sollen)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Architekturmodell finden
+A3: UML auf den neuesten Stand bringen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1:Campus zeichnen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -755,6 +716,40 @@
       <t>A2: Textausgabe
 A3: Funktion für Übergabewerte von Haus und Ebene wegen offset überprüfen</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: je nach ergebnissen von David (Ziel2, GUI, A1) Buttons designen oder eben nicht
+A2: genauerer Designentwurf als das was im Pflichtenheft vorhanden ist, Absprache mit Eric - wird auf Ziel 4 verschoben, da ich es sinnvoller finde, mich dem anzupassen, was Eric schon gemacht hat, als erstmal parallel was neues zu erfinden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: Startbildschirm entwerfen</t>
+    </r>
+  </si>
+  <si>
+    <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
   </si>
 </sst>
 </file>
@@ -1393,6 +1388,51 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1410,51 +1450,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1827,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1855,7 @@
     </row>
     <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1917,11 +1912,11 @@
       <c r="E6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="71"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="22"/>
     </row>
     <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -1935,11 +1930,11 @@
       <c r="E7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="68"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="83"/>
       <c r="I7" s="24"/>
     </row>
     <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1953,11 +1948,11 @@
       <c r="E8" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="72"/>
-      <c r="H8" s="73"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
       <c r="I8" s="24"/>
     </row>
     <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -1971,11 +1966,11 @@
       <c r="E9" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="74" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="72"/>
-      <c r="H9" s="73"/>
+      <c r="F9" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
       <c r="I9" s="46"/>
     </row>
     <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -1989,11 +1984,11 @@
       <c r="E10" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83"/>
       <c r="I10" s="24"/>
     </row>
     <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2007,11 +2002,11 @@
       <c r="E11" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="83"/>
       <c r="I11" s="24"/>
     </row>
     <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2021,11 +2016,11 @@
       <c r="E12" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="83"/>
       <c r="I12" s="24"/>
     </row>
     <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -2035,11 +2030,11 @@
       <c r="E13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="66" t="s">
+      <c r="F13" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="83"/>
       <c r="I13" s="24"/>
     </row>
     <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2086,11 +2081,11 @@
       <c r="E16" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="79"/>
-      <c r="H16" s="80"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="74"/>
       <c r="I16" s="25"/>
     </row>
     <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
@@ -2098,17 +2093,17 @@
         <v>6</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
+      <c r="F17" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="24"/>
     </row>
     <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
@@ -2116,35 +2111,35 @@
         <v>7</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="83"/>
+      <c r="F18" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
       <c r="I18" s="24"/>
     </row>
     <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
       <c r="B19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="46" t="s">
-        <v>50</v>
+      <c r="C19" s="49" t="s">
+        <v>69</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="74" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="72"/>
-      <c r="H19" s="73"/>
+      <c r="F19" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
       <c r="I19" s="24"/>
     </row>
     <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
@@ -2152,35 +2147,35 @@
         <v>23</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
+      <c r="F20" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="82"/>
+      <c r="H20" s="83"/>
       <c r="I20" s="24"/>
     </row>
     <row r="21" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="48"/>
       <c r="E21" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="72"/>
-      <c r="H21" s="73"/>
+        <v>52</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
       <c r="I21" s="24"/>
     </row>
     <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
@@ -2192,13 +2187,13 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="73"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="24"/>
     </row>
     <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2212,11 +2207,11 @@
       <c r="E23" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" s="72"/>
-      <c r="H23" s="73"/>
+      <c r="F23" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
       <c r="I23" s="24"/>
     </row>
     <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2263,11 +2258,11 @@
       <c r="E26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="78" t="s">
+      <c r="F26" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="79"/>
-      <c r="H26" s="80"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="25"/>
     </row>
     <row r="27" spans="2:12" ht="61.8" x14ac:dyDescent="0.25">
@@ -2275,15 +2270,15 @@
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="86"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
     <row r="28" spans="2:12" ht="41.4" x14ac:dyDescent="0.25">
@@ -2291,15 +2286,15 @@
         <v>7</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="75"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="77"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="24"/>
     </row>
     <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2307,17 +2302,17 @@
         <v>8</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="74" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="72"/>
-      <c r="H29" s="73"/>
+      <c r="F29" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
       <c r="I29" s="24"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -2325,7 +2320,7 @@
         <v>22</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,6 +2447,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F16:H16"/>
@@ -2464,14 +2467,6 @@
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">

</xml_diff>

<commit_message>
David: GUI: ProgressBar für Splashscreen hinzugefügt; Optionenmenü umgesetzt xml: Kommentare hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
+++ b/Dokumente/Organisation/Plan der Wochenziele UASJ-Maps.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="552" yWindow="120" windowWidth="13620" windowHeight="8256"/>
+    <workbookView xWindow="555" yWindow="120" windowWidth="13620" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Wochenpläne" sheetId="1" r:id="rId1"/>
@@ -113,6 +113,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="C27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A2 hängt an GUI Ziel3 A3
+wobei ausgrauen implementiert ist, wieder anzeigen hingegen nicht</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -290,74 +315,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>A4: Menüführung fertig machen</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>A1: Ausfühliche Recherche wie werden einzelne Test (Klassentest, Modultests &amp; Integrationstest) konkret umgesetzt</t>
     </r>
     <r>
@@ -414,30 +371,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>A1: Logo und Startupscreen reinbringen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color indexed="23"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-A2: ausgegraute Buttons 
-A3: Optionenmenü umsetzen
-A4: Initialzoom in Go-Button implementieren
-A5: David: Test: Sind Räume von RommSpinner auch alle in Datenbank?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>A1: csv datei für Haus 5 anlegen (Knoten eintragen)</t>
     </r>
     <r>
@@ -750,17 +683,146 @@
   </si>
   <si>
     <t>A1: restliche Klassentests nach Vorarbeit in Ziel 2 QA vorbereiten, nicht vergessen - absprache mit jeweiligen Klassenverantwortlichen halten</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Thomas Multitouch, Singletouch (siehe Ziel3 A1 von GO)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A2: Ansteuerung GO feritg machen (restliche setFloor()-Befehle umsetzen (Häuser auf Campus)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A3: David: Singletouch für Campusdarstellung erstellen: Wo wurde gedrückt?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A4: Menüführung fertig machen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A1: Logo und Startupscreen reinbringen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">A2: ausgegraute Buttons </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A3: Optionenmenü umsetzen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="23"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+A4: Initialzoom in Go-Button implementieren
+A5: David: Test: Sind Räume von RommSpinner auch alle in Datenbank?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A6: Progressbar für SplashScreen erstellen</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d\a\t\um\,\ \k\u\r\z"/>
     <numFmt numFmtId="165" formatCode="\Fes\t"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1534,7 +1596,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
     <a:clrScheme name="Larissa">
       <a:dk1>
@@ -1608,7 +1670,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1643,7 +1704,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Larissa">
@@ -1819,27 +1879,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.88671875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.85546875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="43.5" customHeight="1">
       <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1853,7 +1913,7 @@
       <c r="H2" s="3"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="21" customHeight="1">
       <c r="B3" s="10" t="s">
         <v>53</v>
       </c>
@@ -1873,7 +1933,7 @@
       </c>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B4" s="9"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
@@ -1883,7 +1943,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="2:14" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="15.95" customHeight="1">
       <c r="B5" s="38" t="s">
         <v>3</v>
       </c>
@@ -1901,7 +1961,7 @@
       <c r="H5" s="40"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B6" s="43" t="s">
         <v>5</v>
       </c>
@@ -1919,7 +1979,7 @@
       <c r="H6" s="86"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="22.5">
       <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
@@ -1937,7 +1997,7 @@
       <c r="H7" s="83"/>
       <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="2:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="60" customHeight="1">
       <c r="B8" s="47" t="s">
         <v>7</v>
       </c>
@@ -1955,7 +2015,7 @@
       <c r="H8" s="71"/>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="2:14" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="111" customHeight="1">
       <c r="B9" s="47" t="s">
         <v>8</v>
       </c>
@@ -1967,13 +2027,13 @@
         <v>8</v>
       </c>
       <c r="F9" s="69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="70"/>
       <c r="H9" s="71"/>
       <c r="I9" s="46"/>
     </row>
-    <row r="10" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="39" customHeight="1">
       <c r="B10" s="47" t="s">
         <v>15</v>
       </c>
@@ -1991,7 +2051,7 @@
       <c r="H10" s="83"/>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="2:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="50.25" customHeight="1">
       <c r="B11" s="47" t="s">
         <v>17</v>
       </c>
@@ -2009,7 +2069,7 @@
       <c r="H11" s="83"/>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="2:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="37.5" customHeight="1">
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="D12" s="26"/>
@@ -2023,7 +2083,7 @@
       <c r="H12" s="83"/>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="2:14" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="39" customHeight="1">
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
       <c r="D13" s="26"/>
@@ -2037,7 +2097,7 @@
       <c r="H13" s="83"/>
       <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
       <c r="D14" s="26"/>
@@ -2047,7 +2107,7 @@
       <c r="H14" s="24"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B15" s="38" t="s">
         <v>3</v>
       </c>
@@ -2070,7 +2130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="17.100000000000001" customHeight="1">
       <c r="B16" s="43" t="s">
         <v>5</v>
       </c>
@@ -2088,48 +2148,48 @@
       <c r="H16" s="74"/>
       <c r="I16" s="25"/>
     </row>
-    <row r="17" spans="2:12" ht="81.599999999999994" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="101.25">
       <c r="B17" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="47" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="69" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="70"/>
       <c r="H17" s="71"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="132.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="146.25">
       <c r="B18" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="75" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G18" s="76"/>
       <c r="H18" s="77"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="30.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="45">
       <c r="B19" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="47" t="s">
@@ -2142,25 +2202,25 @@
       <c r="H19" s="71"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="91.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="101.25">
       <c r="B20" s="47" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="48"/>
       <c r="E20" s="47" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="81" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G20" s="82"/>
       <c r="H20" s="83"/>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="57.75" customHeight="1">
       <c r="B21" s="56" t="s">
         <v>52</v>
       </c>
@@ -2172,13 +2232,13 @@
         <v>52</v>
       </c>
       <c r="F21" s="69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G21" s="70"/>
       <c r="H21" s="71"/>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="20.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="22.5">
       <c r="B22" s="47" t="s">
         <v>36</v>
       </c>
@@ -2190,13 +2250,13 @@
         <v>50</v>
       </c>
       <c r="F22" s="81" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="82"/>
       <c r="H22" s="83"/>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="68.25" customHeight="1">
       <c r="B23" s="47" t="s">
         <v>48</v>
       </c>
@@ -2208,13 +2268,13 @@
         <v>22</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G23" s="70"/>
       <c r="H23" s="71"/>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B24" s="27"/>
       <c r="C24" s="28"/>
       <c r="D24" s="26"/>
@@ -2224,7 +2284,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
     </row>
-    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" s="29" customFormat="1" ht="15.95" customHeight="1">
       <c r="B25" s="38" t="s">
         <v>3</v>
       </c>
@@ -2247,7 +2307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B26" s="43" t="s">
         <v>5</v>
       </c>
@@ -2265,12 +2325,12 @@
       <c r="H26" s="74"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="2:12" ht="61.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="79.5">
       <c r="B27" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D27" s="23"/>
       <c r="E27" s="47" t="s">
@@ -2281,12 +2341,12 @@
       <c r="H27" s="80"/>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="45.75">
       <c r="B28" s="47" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="47" t="s">
@@ -2297,39 +2357,39 @@
       <c r="H28" s="68"/>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="21.75" customHeight="1">
       <c r="B29" s="47" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="47" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G29" s="70"/>
       <c r="H29" s="71"/>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12">
       <c r="B30" s="56" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="65" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="17.100000000000001" customHeight="1">
       <c r="B32" s="24"/>
     </row>
-    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B33" s="57" t="s">
         <v>27</v>
       </c>
@@ -2337,7 +2397,7 @@
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
     </row>
-    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" ht="17.100000000000001" customHeight="1">
       <c r="B34" s="57" t="s">
         <v>47</v>
       </c>
@@ -2347,7 +2407,7 @@
       <c r="H34" s="51"/>
       <c r="I34" s="52"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9">
       <c r="B35" s="57" t="s">
         <v>28</v>
       </c>
@@ -2356,7 +2416,7 @@
       <c r="E35" s="57"/>
       <c r="H35" s="53"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9">
       <c r="B36" s="57" t="s">
         <v>44</v>
       </c>
@@ -2366,7 +2426,7 @@
       <c r="H36" s="54"/>
       <c r="I36" s="52"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9">
       <c r="B37" s="57" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2435,7 @@
       <c r="E37" s="57"/>
       <c r="I37" s="55"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9">
       <c r="B38" s="57" t="s">
         <v>30</v>
       </c>
@@ -2383,13 +2443,13 @@
       <c r="D38" s="57"/>
       <c r="E38" s="57"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9">
       <c r="B39" s="57"/>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
       <c r="E39" s="57"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9">
       <c r="B40" s="57" t="s">
         <v>38</v>
       </c>
@@ -2397,7 +2457,7 @@
       <c r="D40" s="57"/>
       <c r="E40" s="57"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9">
       <c r="B41" s="58" t="s">
         <v>39</v>
       </c>
@@ -2407,7 +2467,7 @@
       <c r="D41" s="57"/>
       <c r="E41" s="57"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9">
       <c r="B42" s="60" t="s">
         <v>41</v>
       </c>
@@ -2417,7 +2477,7 @@
       <c r="D42" s="57"/>
       <c r="E42" s="57"/>
     </row>
-    <row r="43" spans="2:9" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" ht="51">
       <c r="B43" s="61" t="s">
         <v>43</v>
       </c>
@@ -2427,19 +2487,19 @@
       <c r="D43" s="57"/>
       <c r="E43" s="57"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9">
       <c r="B44" s="57"/>
       <c r="C44" s="57"/>
       <c r="D44" s="57"/>
       <c r="E44" s="57"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9">
       <c r="B45" s="57"/>
       <c r="C45" s="57"/>
       <c r="D45" s="57"/>
       <c r="E45" s="57"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9">
       <c r="B46" s="57"/>
       <c r="C46" s="57"/>
       <c r="D46" s="57"/>

</xml_diff>